<commit_message>
MASTER: Fix Fisher LDA.
</commit_message>
<xml_diff>
--- a/src/bayes.xlsx
+++ b/src/bayes.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Normalization function</t>
   </si>
@@ -43,6 +43,129 @@
   </si>
   <si>
     <t>F-measure</t>
+  </si>
+  <si>
+    <t>Normalization function</t>
+  </si>
+  <si>
+    <t>zscore</t>
+  </si>
+  <si>
+    <t>norm</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>blues</t>
+  </si>
+  <si>
+    <t>classical</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>hiphop</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>reggae</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>blues</t>
+  </si>
+  <si>
+    <t>classical</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>hiphop</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>reggae</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>blues</t>
+  </si>
+  <si>
+    <t>classical</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>disco</t>
+  </si>
+  <si>
+    <t>hiphop</t>
+  </si>
+  <si>
+    <t>jazz</t>
+  </si>
+  <si>
+    <t>metal</t>
+  </si>
+  <si>
+    <t>pop</t>
+  </si>
+  <si>
+    <t>reggae</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>F-measure</t>
+  </si>
+  <si>
+    <t>AUC</t>
   </si>
 </sst>
 </file>
@@ -88,46 +211,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="true"/>
-    <col min="2" max="2" width="5.5703125" customWidth="true"/>
+    <col min="2" max="2" width="8.28515625" customWidth="true"/>
     <col min="3" max="3" width="12.7109375" customWidth="true"/>
     <col min="4" max="4" width="12.7109375" customWidth="true"/>
     <col min="5" max="5" width="13.7109375" customWidth="true"/>
     <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="12.7109375" customWidth="true"/>
+    <col min="8" max="8" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="C2" s="0">
         <v>0</v>
       </c>
@@ -143,12 +272,17 @@
       <c r="G2" s="0">
         <v>0.90277777777777779</v>
       </c>
+      <c r="H2" s="0">
+        <v>0.48472222222222222</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="C3" s="0">
         <v>0.10062893081761007</v>
       </c>
@@ -164,12 +298,17 @@
       <c r="G3" s="0">
         <v>0.97945205479452058</v>
       </c>
+      <c r="H3" s="0">
+        <v>0.9376535626535627</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="0">
         <v>0</v>
       </c>
@@ -185,12 +324,17 @@
       <c r="G4" s="0">
         <v>0.89583333333333337</v>
       </c>
+      <c r="H4" s="0">
+        <v>0.44791666666666669</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="C5" s="0">
         <v>0.10062893081761007</v>
       </c>
@@ -206,12 +350,17 @@
       <c r="G5" s="0">
         <v>0.88732394366197187</v>
       </c>
+      <c r="H5" s="0">
+        <v>0.47631578947368419</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="0">
         <v>0.025157232704402517</v>
       </c>
@@ -227,12 +376,17 @@
       <c r="G6" s="0">
         <v>0.91034482758620683</v>
       </c>
+      <c r="H6" s="0">
+        <v>0.49051633298208641</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" s="0">
         <v>0</v>
       </c>
@@ -248,12 +402,17 @@
       <c r="G7" s="0">
         <v>0.90277777777777779</v>
       </c>
+      <c r="H7" s="0">
+        <v>0.48472222222222222</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>21</v>
+      </c>
       <c r="C8" s="0">
         <v>0.22641509433962265</v>
       </c>
@@ -269,12 +428,17 @@
       <c r="G8" s="0">
         <v>0.87943262411347511</v>
       </c>
+      <c r="H8" s="0">
+        <v>0.47308488612836441</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
       <c r="C9" s="0">
         <v>0.3081761006289308</v>
       </c>
@@ -290,12 +454,17 @@
       <c r="G9" s="0">
         <v>0.86832740213523119</v>
       </c>
+      <c r="H9" s="0">
+        <v>0.44525547445255476</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="0">
         <v>0.025157232704402517</v>
       </c>
@@ -311,12 +480,17 @@
       <c r="G10" s="0">
         <v>0.88811188811188801</v>
       </c>
+      <c r="H10" s="0">
+        <v>0.44718309859154931</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="0"/>
+        <v>11</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="0">
         <v>0.10062893081761007</v>
       </c>
@@ -332,12 +506,17 @@
       <c r="G11" s="0">
         <v>0.91095890410958913</v>
       </c>
+      <c r="H11" s="0">
+        <v>0.44932432432432434</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="0">
         <v>0.22641509433962265</v>
       </c>
@@ -353,12 +532,17 @@
       <c r="G12" s="0">
         <v>0.84328358208955223</v>
       </c>
+      <c r="H12" s="0">
+        <v>0.50331785003317853</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="C13" s="0">
         <v>1.6100628930817611</v>
       </c>
@@ -374,12 +558,17 @@
       <c r="G13" s="0">
         <v>0.93525179856115104</v>
       </c>
+      <c r="H13" s="0">
+        <v>0.90051020408163263</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="C14" s="0">
         <v>1.0628930817610063</v>
       </c>
@@ -395,12 +584,17 @@
       <c r="G14" s="0">
         <v>0.84363636363636374</v>
       </c>
+      <c r="H14" s="0">
+        <v>0.40277777777777779</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="C15" s="0">
         <v>0.76100628930817615</v>
       </c>
@@ -416,12 +610,17 @@
       <c r="G15" s="0">
         <v>0.8424908424908425</v>
       </c>
+      <c r="H15" s="0">
+        <v>0.43434134217067111</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="C16" s="0">
         <v>0.76100628930817615</v>
       </c>
@@ -437,12 +636,17 @@
       <c r="G16" s="0">
         <v>0.84981684981684991</v>
       </c>
+      <c r="H16" s="0">
+        <v>0.46727423363711684</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="C17" s="0">
         <v>0.50943396226415094</v>
       </c>
@@ -458,12 +662,17 @@
       <c r="G17" s="0">
         <v>0.87084870848708473</v>
       </c>
+      <c r="H17" s="0">
+        <v>0.57932330827067668</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>31</v>
+      </c>
       <c r="C18" s="0">
         <v>1.8176100628930818</v>
       </c>
@@ -479,12 +688,17 @@
       <c r="G18" s="0">
         <v>0.88172043010752688</v>
       </c>
+      <c r="H18" s="0">
+        <v>0.55190417690417692</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="C19" s="0">
         <v>1.2327044025157232</v>
       </c>
@@ -500,12 +714,17 @@
       <c r="G19" s="0">
         <v>0.84782608695652162</v>
       </c>
+      <c r="H19" s="0">
+        <v>0.40344827586206899</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B20" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>33</v>
+      </c>
       <c r="C20" s="0">
         <v>0.62893081761006286</v>
       </c>
@@ -521,12 +740,17 @@
       <c r="G20" s="0">
         <v>0.83088235294117652</v>
       </c>
+      <c r="H20" s="0">
+        <v>0.400709219858156</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="0"/>
+        <v>12</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="C21" s="0">
         <v>1.2327044025157232</v>
       </c>
@@ -542,12 +766,17 @@
       <c r="G21" s="0">
         <v>0.85507246376811596</v>
       </c>
+      <c r="H21" s="0">
+        <v>0.44261083743842361</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="0">
         <v>1.2327044025157232</v>
       </c>
@@ -563,12 +792,17 @@
       <c r="G22" s="0">
         <v>0.83941605839416067</v>
       </c>
+      <c r="H22" s="0">
+        <v>0.39930555555555558</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>36</v>
+      </c>
       <c r="C23" s="0">
         <v>0.76100628930817615</v>
       </c>
@@ -584,12 +818,17 @@
       <c r="G23" s="0">
         <v>0.94464944649446492</v>
       </c>
+      <c r="H23" s="0">
+        <v>0.89834515366430245</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>37</v>
+      </c>
       <c r="C24" s="0">
         <v>0.76100628930817615</v>
       </c>
@@ -605,12 +844,17 @@
       <c r="G24" s="0">
         <v>0.82656826568265696</v>
       </c>
+      <c r="H24" s="0">
+        <v>0.3971631205673759</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>38</v>
+      </c>
       <c r="C25" s="0">
         <v>2.0377358490566038</v>
       </c>
@@ -626,12 +870,17 @@
       <c r="G25" s="0">
         <v>0.85611510791366907</v>
       </c>
+      <c r="H25" s="0">
+        <v>0.40202702702702703</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="C26" s="0">
         <v>0.90566037735849059</v>
       </c>
@@ -647,12 +896,17 @@
       <c r="G26" s="0">
         <v>0.83088235294117641</v>
       </c>
+      <c r="H26" s="0">
+        <v>0.397887323943662</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="C27" s="0">
         <v>2.0377358490566038</v>
       </c>
@@ -668,12 +922,17 @@
       <c r="G27" s="0">
         <v>0.88489208633093519</v>
       </c>
+      <c r="H27" s="0">
+        <v>0.59735872235872245</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>41</v>
+      </c>
       <c r="C28" s="0">
         <v>2.2704402515723272</v>
       </c>
@@ -689,12 +948,17 @@
       <c r="G28" s="0">
         <v>0.87455197132616491</v>
       </c>
+      <c r="H28" s="0">
+        <v>0.50939597315436236</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B29" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>42</v>
+      </c>
       <c r="C29" s="0">
         <v>0.62893081761006286</v>
       </c>
@@ -710,12 +974,17 @@
       <c r="G29" s="0">
         <v>0.82962962962962972</v>
       </c>
+      <c r="H29" s="0">
+        <v>0.4263157894736842</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>43</v>
+      </c>
       <c r="C30" s="0">
         <v>1.0628930817610063</v>
       </c>
@@ -731,12 +1000,17 @@
       <c r="G30" s="0">
         <v>0.84981684981684991</v>
       </c>
+      <c r="H30" s="0">
+        <v>0.46809440559440568</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B31" s="0"/>
+        <v>13</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="C31" s="0">
         <v>0.15723270440251572</v>
       </c>
@@ -751,6 +1025,9 @@
       </c>
       <c r="G31" s="0">
         <v>0.83018867924528295</v>
+      </c>
+      <c r="H31" s="0">
+        <v>0.49074074074074081</v>
       </c>
     </row>
   </sheetData>

</xml_diff>